<commit_message>
2024 AGU Commit - 5um data and analysis
Data (5um) set from Glenn Orton plus many processing changes and updates to accommodate analysis. Added the ability to make L2 (absorption) map plots (pngs). Also added the ability to incorporate 5um data (FITS) into both L2 and L3 maps. There's a residual capability to incorporate 5um png maps from ALPO-Japan that could be generalized to any maps from ALPO-Japan. This would be very useful for instance for 889 nm CH4 maps and for NUV maps.
</commit_message>
<xml_diff>
--- a/5micron/5umCatalog-static.xlsx
+++ b/5micron/5umCatalog-static.xlsx
@@ -8,14 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Astronomy\Projects\SAS 2021 Ammonia\Jupiter_NH3_Analysis_P3\5micron\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{08C14E8B-2132-47C3-9324-A82862040460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A056CE1E-3CD3-4501-BDF5-9C24EFBAC55A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{9C9EFB5B-4177-442D-8F55-DB5ECBE49F71}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{9C9EFB5B-4177-442D-8F55-DB5ECBE49F71}"/>
   </bookViews>
   <sheets>
     <sheet name="5umCatalog" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -706,11 +719,11 @@
     <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="38" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="39" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="40" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="16" fillId="39" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="16" fillId="38" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1089,8 +1102,8 @@
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B27" sqref="B27:F29"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1769,7 +1782,7 @@
       <c r="A20" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="13">
+      <c r="B20" s="17">
         <v>45213.471018518518</v>
       </c>
       <c r="C20" s="12">
@@ -1804,7 +1817,7 @@
       <c r="A21" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B21" s="13">
+      <c r="B21" s="17">
         <v>45213.528113425928</v>
       </c>
       <c r="C21" s="12">
@@ -1839,7 +1852,7 @@
       <c r="A22" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="13">
+      <c r="B22" s="17">
         <v>45213.620150462964</v>
       </c>
       <c r="C22" s="12">
@@ -1870,248 +1883,248 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B23" s="15">
+    <row r="23" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="16">
         <v>45214.445555555554</v>
       </c>
-      <c r="C23" s="14">
+      <c r="C23" s="13">
         <v>10.5</v>
       </c>
-      <c r="D23" s="14">
+      <c r="D23" s="13">
         <v>297.8</v>
       </c>
-      <c r="E23" s="14">
+      <c r="E23" s="13">
         <v>330.5</v>
       </c>
-      <c r="F23" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G23" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="H23" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="I23" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="J23" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="K23" s="14" t="s">
+      <c r="F23" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="H23" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="I23" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="J23" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="K23" s="13" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B24" s="15">
+    <row r="24" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="16">
         <v>45214.501319444447</v>
       </c>
-      <c r="C24" s="14">
+      <c r="C24" s="13">
         <v>59.5</v>
       </c>
-      <c r="D24" s="14">
+      <c r="D24" s="13">
         <v>346.4</v>
       </c>
-      <c r="E24" s="14">
+      <c r="E24" s="13">
         <v>19</v>
       </c>
-      <c r="F24" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G24" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="H24" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="I24" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="J24" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="K24" s="14" t="s">
+      <c r="F24" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="H24" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="I24" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="J24" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="K24" s="13" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B25" s="15">
+    <row r="25" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="16">
         <v>45214.606111111112</v>
       </c>
-      <c r="C25" s="14">
+      <c r="C25" s="13">
         <v>151.5</v>
       </c>
-      <c r="D25" s="14">
+      <c r="D25" s="13">
         <v>77.599999999999994</v>
       </c>
-      <c r="E25" s="14">
+      <c r="E25" s="13">
         <v>110.3</v>
       </c>
-      <c r="F25" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G25" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="H25" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="I25" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="J25" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="K25" s="14" t="s">
+      <c r="F25" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="H25" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="I25" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="J25" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="K25" s="13" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B26" s="15">
+    <row r="26" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="16">
         <v>45214.63826388889</v>
       </c>
-      <c r="C26" s="14">
+      <c r="C26" s="13">
         <v>179.7</v>
       </c>
-      <c r="D26" s="14">
+      <c r="D26" s="13">
         <v>105.6</v>
       </c>
-      <c r="E26" s="14">
+      <c r="E26" s="13">
         <v>138.30000000000001</v>
       </c>
-      <c r="F26" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G26" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="H26" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="I26" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="J26" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="K26" s="14" t="s">
+      <c r="F26" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G26" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="H26" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="I26" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="J26" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="K26" s="13" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B27" s="17">
+    <row r="27" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="15">
         <v>45327.013402777775</v>
       </c>
-      <c r="C27" s="16">
+      <c r="C27" s="14">
         <v>193.3</v>
       </c>
-      <c r="D27" s="16">
+      <c r="D27" s="14">
         <v>341.8</v>
       </c>
-      <c r="E27" s="16">
+      <c r="E27" s="14">
         <v>44.4</v>
       </c>
-      <c r="F27" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="G27" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="H27" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="I27" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="J27" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="K27" s="16" t="s">
+      <c r="F27" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G27" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="H27" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="I27" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="J27" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="K27" s="14" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B28" s="17">
+    <row r="28" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" s="15">
         <v>45327.061307870368</v>
       </c>
-      <c r="C28" s="16">
+      <c r="C28" s="14">
         <v>235.4</v>
       </c>
-      <c r="D28" s="16">
+      <c r="D28" s="14">
         <v>23.5</v>
       </c>
-      <c r="E28" s="16">
+      <c r="E28" s="14">
         <v>86.1</v>
       </c>
-      <c r="F28" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="G28" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="H28" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="I28" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="J28" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="K28" s="16" t="s">
+      <c r="F28" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G28" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="H28" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="I28" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="J28" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="K28" s="14" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B29" s="17">
+    <row r="29" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="15">
         <v>45327.162233796298</v>
       </c>
-      <c r="C29" s="16">
+      <c r="C29" s="14">
         <v>324</v>
       </c>
-      <c r="D29" s="16">
+      <c r="D29" s="14">
         <v>111.3</v>
       </c>
-      <c r="E29" s="16">
+      <c r="E29" s="14">
         <v>173.9</v>
       </c>
-      <c r="F29" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="G29" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="H29" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="I29" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="J29" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="K29" s="16" t="s">
+      <c r="F29" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G29" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="H29" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="I29" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="J29" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="K29" s="14" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>